<commit_message>
adds example of a runtime test
</commit_message>
<xml_diff>
--- a/src/n-excel/N/Package/Excel/Editor/ExcelTestsDocument.xlsx
+++ b/src/n-excel/N/Package/Excel/Editor/ExcelTestsDocument.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doug/dev/now/unity-insurance-dungeon/Assets/Story/Chapter1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doug/dev/now/unity-n-excel/test/Assets/pkg-all/n-excel/N/Package/Excel/Editor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADA50DA-BA8A-9C4A-8110-5DD1E4647738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33EE861-E7F8-1145-952B-1B879DC8CD8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="1800" windowWidth="38400" windowHeight="21960" xr2:uid="{BDC72600-1FBC-B949-999E-EBC59978050C}"/>
+    <workbookView xWindow="11640" yWindow="5900" windowWidth="38400" windowHeight="21960" xr2:uid="{BDC72600-1FBC-B949-999E-EBC59978050C}"/>
   </bookViews>
   <sheets>
     <sheet name="Mancy" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet 1" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
+    <sheet name="Hello" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +34,7 @@
     <author>doug</author>
   </authors>
   <commentList>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{2D4D2001-84EA-8547-BE7A-9181AA33EFB5}">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{2D4D2001-84EA-8547-BE7A-9181AA33EFB5}">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>character</t>
   </si>
@@ -174,6 +174,21 @@
   </si>
   <si>
     <t>Ok, bye!</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>case: new case</t>
   </si>
 </sst>
 </file>
@@ -262,7 +277,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -279,6 +294,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -595,59 +616,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30392611-C834-F04E-A0B6-ECA02D6148E7}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
+      <c r="K1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>1</v>
       </c>
@@ -660,21 +681,24 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="H2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3">
@@ -689,19 +713,19 @@
       <c r="E3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>1</v>
+      </c>
       <c r="G3" s="3"/>
-      <c r="H3" t="s">
+      <c r="H3" s="3"/>
+      <c r="I3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
-        <v>1</v>
-      </c>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>1</v>
       </c>
@@ -714,21 +738,21 @@
       <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>2</v>
-      </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>1</v>
       </c>
@@ -741,19 +765,19 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
       <c r="G6" s="3"/>
-      <c r="H6" t="s">
+      <c r="H6" s="3"/>
+      <c r="I6" t="s">
         <v>4</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
-        <v>1</v>
-      </c>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>1</v>
       </c>
@@ -766,246 +790,249 @@
       <c r="E7" s="3">
         <v>1</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
       <c r="G7" s="3"/>
-      <c r="J7" t="s">
+      <c r="H7" s="3"/>
+      <c r="K7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6">
-        <v>1</v>
-      </c>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <v>1</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="6"/>
+      <c r="I8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="K8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="7"/>
       <c r="M8" s="7"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="6">
-        <v>1</v>
-      </c>
+      <c r="N8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="6">
         <v>1</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6"/>
+      <c r="I9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-      <c r="K9" s="7" t="s">
+      <c r="K9" s="7"/>
+      <c r="L9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="7"/>
       <c r="M9" s="7"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="6">
-        <v>1</v>
-      </c>
+      <c r="N9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="6">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
         <v>0</v>
       </c>
-      <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6"/>
+      <c r="I10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="7"/>
+      <c r="L10" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="7"/>
       <c r="M10" s="7"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="6">
+      <c r="N10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="6">
         <v>0</v>
       </c>
-      <c r="B11" s="6">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6">
+        <v>1</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-      <c r="K11" s="7" t="s">
+      <c r="K11" s="7"/>
+      <c r="L11" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L11" s="7"/>
       <c r="M11" s="7"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="N11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-      <c r="K12" s="7" t="s">
+      <c r="K12" s="7"/>
+      <c r="L12" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="M12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="M12" s="7"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
+      <c r="N12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="7" t="s">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L13" s="7" t="s">
+      <c r="M13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="M13" s="7"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="N13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="H14" s="3"/>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
         <v>20</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
-      <c r="H15" t="s">
+      <c r="H15" s="3"/>
+      <c r="I15" t="s">
         <v>4</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-      <c r="H16" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="1" t="s">
+      <c r="H16" s="3"/>
+      <c r="I16" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" t="s">
+      <c r="H17" s="3"/>
+      <c r="I17" t="s">
         <v>4</v>
       </c>
-      <c r="K17" s="1"/>
-      <c r="L17" t="s">
+      <c r="L17" s="1"/>
+      <c r="M17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-      <c r="H18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="2" t="s">
+      <c r="H18" s="3"/>
+      <c r="I18" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="G20" s="3"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="6">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="H20" s="3"/>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="6">
         <v>0</v>
       </c>
-      <c r="B24" s="6">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="C24" s="6">
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
         <v>4</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>28</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1032,29 +1059,10 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>A5:G18</xm:sqref>
+          <xm:sqref>B5:H18</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="10" id="{FAB5B07F-89B0-D64C-806D-E16E0C8BED1E}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
-              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>F2:F3</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="9" id="{18790FB7-E4F6-3347-B932-34B94EC7800F}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1073,7 +1081,7 @@
           <xm:sqref>G2:G3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{680EB9AE-66CF-E644-B829-C63952D48F8E}">
+          <x14:cfRule type="iconSet" priority="9" id="{18790FB7-E4F6-3347-B932-34B94EC7800F}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1089,10 +1097,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>G20</xm:sqref>
+          <xm:sqref>H2:H3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{ED6FB7DF-24FD-204F-BE50-BBAF9E90933F}">
+          <x14:cfRule type="iconSet" priority="8" id="{680EB9AE-66CF-E644-B829-C63952D48F8E}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1108,10 +1116,10 @@
               <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>A3</xm:sqref>
+          <xm:sqref>H20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{F48C3DA9-B6F8-7543-8845-524D92C19934}">
+          <x14:cfRule type="iconSet" priority="7" id="{ED6FB7DF-24FD-204F-BE50-BBAF9E90933F}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1130,7 +1138,7 @@
           <xm:sqref>B3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{531934EA-4B62-264F-A2D8-2DA522AE7A4F}">
+          <x14:cfRule type="iconSet" priority="6" id="{F48C3DA9-B6F8-7543-8845-524D92C19934}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1149,7 +1157,7 @@
           <xm:sqref>C3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{05D17AE3-B03B-A74D-8FB2-EDDFD33A4559}">
+          <x14:cfRule type="iconSet" priority="5" id="{531934EA-4B62-264F-A2D8-2DA522AE7A4F}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1168,6 +1176,25 @@
           <xm:sqref>D3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{05D17AE3-B03B-A74D-8FB2-EDDFD33A4559}">
+            <x14:iconSet showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="0"/>
+              <x14:cfIcon iconSet="3TrafficLights1" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>E3</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="3" id="{68A679B5-9539-2042-A6D5-8FF910529298}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
@@ -1184,10 +1211,29 @@
               <x14:cfIcon iconSet="3Symbols" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>E3</xm:sqref>
+          <xm:sqref>F3</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="iconSet" priority="2" id="{B7EB9C37-4158-C84A-BD92-5C41E9E868AC}">
+            <x14:iconSet showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C24</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{E5B731E0-2B67-0849-B189-746BCEF70DC0}">
             <x14:iconSet showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -1204,25 +1250,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>B24</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{E5B731E0-2B67-0849-B189-746BCEF70DC0}">
-            <x14:iconSet showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="0"/>
-              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>A24</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1232,12 +1259,481 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2771219B-29C4-564D-8E37-67E1662E621B}">
-  <dimension ref="A1"/>
+  <dimension ref="B2:H42"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="5" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="9">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="9">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>3</v>
+      </c>
+      <c r="G5" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="E16" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="E18" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9">
+        <v>2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="E22" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="E26" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>2</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2</v>
+      </c>
+      <c r="E30" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <v>2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="9">
+        <v>1</v>
+      </c>
+      <c r="C32" s="9">
+        <v>2</v>
+      </c>
+      <c r="E32" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
+        <v>2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9">
+        <v>2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="C36" s="9">
+        <v>2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="C37" s="9">
+        <v>2</v>
+      </c>
+      <c r="E37" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="9">
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2</v>
+      </c>
+      <c r="E39" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
+        <v>2</v>
+      </c>
+      <c r="E41" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>2</v>
+      </c>
+      <c r="E42" s="9">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1246,7 +1742,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BAA31DD-46AB-144B-83D9-AE7686205E76}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>